<commit_message>
addition of powerpoints and timelog
</commit_message>
<xml_diff>
--- a/timelog.xlsx
+++ b/timelog.xlsx
@@ -5,23 +5,57 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dtsyn\byu\cs479_testFiles\AAAFinalProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dtsyn\byu\cs479_testFiles\AAAFinalProject\479_Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5366FB-D2E0-414F-B45E-1E6ED3B83FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39F7B1A-F8A9-4C27-B29B-708536711666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>hours</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">finding documents and coming up with a proposal and reviewing </t>
+  </si>
+  <si>
+    <t>Making the powerpoint, continuing to refine proposal, document reviewal</t>
+  </si>
+  <si>
+    <t>total hours</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -55,8 +89,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -337,12 +377,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="25.77734375" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>45965</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1">
+        <f>SUM(B:B)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>45966</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
all of the lines are cleaned and ready to be combined
</commit_message>
<xml_diff>
--- a/timelog.xlsx
+++ b/timelog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dtsyn\byu\cs479_testFiles\AAAFinalProject\479_Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39F7B1A-F8A9-4C27-B29B-708536711666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C06B47-EC0D-48F5-956C-0CADCF94F037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29760" yWindow="960" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>hours</t>
   </si>
@@ -54,6 +54,15 @@
   </si>
   <si>
     <t>total hours</t>
+  </si>
+  <si>
+    <t>Finalizing the powerpoint, finding other articles, and other planing steps</t>
+  </si>
+  <si>
+    <t>beguin cleaning portuguese data 90%</t>
+  </si>
+  <si>
+    <t>finished cleaning the portguese data completely and beguin cleaning papiamento</t>
   </si>
 </sst>
 </file>
@@ -377,15 +386,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" style="1"/>
     <col min="3" max="3" width="25.77734375" style="1" customWidth="1"/>
     <col min="4" max="16384" width="8.88671875" style="1"/>
@@ -417,7 +426,7 @@
       </c>
       <c r="E2" s="1">
         <f>SUM(B:B)</f>
-        <v>2</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -429,6 +438,39 @@
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>45971</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>45978</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>45979</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.75</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to time log and creation of line combiner
</commit_message>
<xml_diff>
--- a/timelog.xlsx
+++ b/timelog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dtsyn\byu\cs479_testFiles\AAAFinalProject\479_Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C06B47-EC0D-48F5-956C-0CADCF94F037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129F615B-BD89-4927-AB59-5BCED0B06217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29760" yWindow="960" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3072" yWindow="3072" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>hours</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>finished cleaning the portguese data completely and beguin cleaning papiamento</t>
+  </si>
+  <si>
+    <t>finished cleaning papiment</t>
+  </si>
+  <si>
+    <t>lableing data and combining it</t>
   </si>
 </sst>
 </file>
@@ -386,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -426,7 +432,7 @@
       </c>
       <c r="E2" s="1">
         <f>SUM(B:B)</f>
-        <v>6.75</v>
+        <v>10.25</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
@@ -471,6 +477,28 @@
       </c>
       <c r="C6" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>45982</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>45982</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>